<commit_message>
Added a README.md Also changed the code that generates the .xlsx so that columns are labeled node1 and node1 instead of src and tar to make it clear that this is for undirected graphs.
</commit_message>
<xml_diff>
--- a/sample_output/sample_output.xlsx
+++ b/sample_output/sample_output.xlsx
@@ -1950,10 +1950,10 @@
     <t>ST8SIA4</t>
   </si>
   <si>
-    <t>src</t>
-  </si>
-  <si>
-    <t>tar</t>
+    <t>node1</t>
+  </si>
+  <si>
+    <t>node2</t>
   </si>
   <si>
     <t>weight</t>

</xml_diff>